<commit_message>
Remove "删除" column from detail view
</commit_message>
<xml_diff>
--- a/codegen/__out__/pc/public/excel_template/base/usr.xlsx
+++ b/codegen/__out__/pc/public/excel_template/base/usr.xlsx
@@ -51,6 +51,9 @@
     <t xml:space="preserve">&lt;%=comment.dept_ids_lbl%&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;%=comment.tenant_id_lbl%&gt;&lt;%selectList.tenant_id = data.findAllTenant.map((item) =&gt; item.lbl)%&gt;&lt;%_dataValidation_({ sqref: `${ _col }2:${ _col }${ _lastRow }`, formula1: `"${ selectList.tenant_id.join(",") }"` })%&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;%=comment.role_ids_lbl%&gt;</t>
   </si>
   <si>
@@ -88,6 +91,9 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;%=model.dept_ids_lbl%&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;%=model.tenant_id_lbl%&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;%=model.role_ids_lbl%&gt;</t>
@@ -476,46 +482,52 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M2" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="N2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>